<commit_message>
feat: solution with Google.OrTools
</commit_message>
<xml_diff>
--- a/nosokomeio.xlsx
+++ b/nosokomeio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoLee\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoLee\source\repos\MedicalShiftProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7362C-ABFF-4682-941E-0D2D8357C1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6B8999-33A9-441D-8257-2684AF91B6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5085" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{230D00FD-D74E-4E7F-B6AD-0424789200CA}"/>
   </bookViews>
@@ -206,7 +206,27 @@
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -559,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5EEA1A-F88C-432A-B611-29BB32E68D9D}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -1097,7 +1117,7 @@
   <dimension ref="A1:JA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,13 +1185,13 @@
         <v>45597</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1183,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1192,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1230,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3">
         <v>0</v>
@@ -1239,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="3">
         <v>0</v>
@@ -1508,16 +1528,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
         <v>0</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -1532,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="5">
         <v>0</v>
@@ -1851,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1860,22 +1880,22 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1884,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:261" x14ac:dyDescent="0.3">
@@ -1898,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1907,22 +1927,22 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1931,7 +1951,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:261" x14ac:dyDescent="0.3">
@@ -1998,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -2013,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -2045,25 +2065,25 @@
         <v>0</v>
       </c>
       <c r="F10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="3">
         <v>0</v>
       </c>
       <c r="K10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="3">
         <v>0</v>
@@ -2341,13 +2361,13 @@
         <v>0</v>
       </c>
       <c r="G11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="5">
         <v>0</v>
@@ -2356,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="5">
         <v>0</v>
@@ -2672,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2681,22 +2701,22 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2705,7 +2725,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:261" x14ac:dyDescent="0.3">
@@ -2719,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2728,22 +2748,22 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -2752,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:261" x14ac:dyDescent="0.3">
@@ -2819,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -2831,13 +2851,13 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -2866,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -2878,13 +2898,13 @@
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="3">
         <v>0</v>
@@ -3171,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="5">
         <v>0</v>
@@ -3493,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -3502,22 +3522,22 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -3526,7 +3546,7 @@
         <v>0</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:261" x14ac:dyDescent="0.3">
@@ -3540,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -3549,22 +3569,22 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -3573,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:261" x14ac:dyDescent="0.3">
@@ -3646,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -3658,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -3675,19 +3695,19 @@
         <v>45619</v>
       </c>
       <c r="B24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
       </c>
       <c r="D24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="3">
         <v>1</v>
@@ -3696,19 +3716,19 @@
         <v>1</v>
       </c>
       <c r="I24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="3">
         <v>0</v>
@@ -3974,13 +3994,13 @@
         <v>1</v>
       </c>
       <c r="D25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="5">
         <v>1</v>
@@ -3989,25 +4009,25 @@
         <v>1</v>
       </c>
       <c r="I25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="5">
         <v>0</v>
       </c>
       <c r="O25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25"/>
       <c r="Q25"/>
@@ -4261,10 +4281,10 @@
         <v>45621</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -4308,13 +4328,13 @@
         <v>45622</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4323,22 +4343,22 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <v>0</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -4347,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:261" x14ac:dyDescent="0.3">
@@ -4355,13 +4375,13 @@
         <v>45623</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -4370,22 +4390,22 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>0</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -4394,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:261" x14ac:dyDescent="0.3">
@@ -4402,10 +4422,10 @@
         <v>45624</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -4449,10 +4469,10 @@
         <v>45625</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -4496,13 +4516,13 @@
         <v>45626</v>
       </c>
       <c r="B31" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="7">
         <v>0</v>
@@ -4786,10 +4806,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:O31">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4803,7 +4823,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="B2" sqref="B2:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: add extra features
- isJunior so they cannot work alone
- set number of shifts per person
- fix shift balancing if not given explicitly
- extra bool to not work back-to-back
- error handling
</commit_message>
<xml_diff>
--- a/nosokomeio.xlsx
+++ b/nosokomeio.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoLee\source\repos\MedicalShiftProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6B8999-33A9-441D-8257-2684AF91B6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7569577-2256-4C81-A3F1-94D1E0070459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5085" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{230D00FD-D74E-4E7F-B6AD-0424789200CA}"/>
+    <workbookView xWindow="-28800" yWindow="5220" windowWidth="28800" windowHeight="15270" xr2:uid="{230D00FD-D74E-4E7F-B6AD-0424789200CA}"/>
   </bookViews>
   <sheets>
     <sheet name="program" sheetId="1" r:id="rId1"/>
     <sheet name="negatives" sheetId="2" r:id="rId2"/>
-    <sheet name="negatives (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="negatives (backup)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,27 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Number of people</t>
   </si>
   <si>
     <t>isWeekend</t>
-  </si>
-  <si>
-    <t>Total required:</t>
-  </si>
-  <si>
-    <t>People available</t>
-  </si>
-  <si>
-    <t>Average per person</t>
-  </si>
-  <si>
-    <t>Weekends total</t>
-  </si>
-  <si>
-    <t>weekend persons</t>
   </si>
   <si>
     <t>ΧΡΙΣΤΟΔΟΥΛΟΥ</t>
@@ -91,6 +76,48 @@
   <si>
     <t>ΠΑΝΑΓΟΥΛΑ</t>
   </si>
+  <si>
+    <t>Total shifts</t>
+  </si>
+  <si>
+    <t>Total Shifts per person</t>
+  </si>
+  <si>
+    <t>Total shifts alocated per person</t>
+  </si>
+  <si>
+    <t>Allow back-to-back shifts</t>
+  </si>
+  <si>
+    <t>Is Junior (cannot work alone)</t>
+  </si>
+  <si>
+    <t>Balance shifts automatically</t>
+  </si>
+  <si>
+    <t>SETTINGS</t>
+  </si>
+  <si>
+    <t>Automatically calculated</t>
+  </si>
+  <si>
+    <t>Total Days</t>
+  </si>
+  <si>
+    <t>ΜΠΑΜΟΠΟΥΛΟΣ</t>
+  </si>
+  <si>
+    <t>Desired shifts per person</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>multiple programs as solutions (3-4)</t>
+  </si>
+  <si>
+    <t>weekend balancing remake</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,13 +135,37 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -193,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -202,31 +253,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -577,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5EEA1A-F88C-432A-B611-29BB32E68D9D}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,522 +622,410 @@
     <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45597</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45598</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45599</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45600</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45601</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45602</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>45603</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>45608</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45609</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45610</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45612</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45613</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45617</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>45618</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>45619</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45620</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>45621</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>45622</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>45624</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>45625</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>45626</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="10">
         <f>COUNTIF(A2:A32,"&lt;&gt;")</f>
         <v>30</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>45597</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <f>C2*B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>45598</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <f>C3*B3</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>45599</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D31" si="0">C4*B4</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>45600</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>45601</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>45602</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>45603</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>45604</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>45605</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>45606</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>45607</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>45608</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>45609</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>45610</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>45611</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>45612</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>45613</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>45614</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>45615</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>45616</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>45617</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>45618</v>
-      </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>45619</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>45620</v>
-      </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>45621</v>
-      </c>
-      <c r="B26">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>45622</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>45623</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>45624</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>45625</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>45626</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="10">
         <f>SUM(B2:B31)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36">
-        <f>B34/B35</f>
-        <v>6.4285714285714288</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38">
-        <f>SUM(D2:D31)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D37" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="10">
+        <f>negatives!B37</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39">
-        <f>B38/B35</f>
-        <v>1.9285714285714286</v>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1114,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3734B0B9-157B-4360-A5C8-B7323A1492CD}">
-  <dimension ref="A1:JA31"/>
+  <dimension ref="A1:JA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,46 +1060,46 @@
   <sheetData>
     <row r="1" spans="1:261" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:261" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4804,12 +4726,120 @@
       <c r="IZ31"/>
       <c r="JA31"/>
     </row>
+    <row r="34" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36">
+        <v>7</v>
+      </c>
+      <c r="J36">
+        <v>7</v>
+      </c>
+      <c r="K36">
+        <v>7</v>
+      </c>
+      <c r="L36">
+        <v>7</v>
+      </c>
+      <c r="M36">
+        <v>7</v>
+      </c>
+      <c r="N36">
+        <v>7</v>
+      </c>
+      <c r="O36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="10">
+        <f>SUM(B36:O36)</f>
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:O31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2:O31 B35:O36">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4823,7 +4853,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O31"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4834,46 +4864,46 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6288,10 +6318,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:O31">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feat: export result to excel workbook
</commit_message>
<xml_diff>
--- a/nosokomeio.xlsx
+++ b/nosokomeio.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoLee\source\repos\MedicalShiftProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7569577-2256-4C81-A3F1-94D1E0070459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F37B5D-CD81-4A2C-9A99-773CCBF433AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5220" windowWidth="28800" windowHeight="15270" xr2:uid="{230D00FD-D74E-4E7F-B6AD-0424789200CA}"/>
+    <workbookView xWindow="-28920" yWindow="5085" windowWidth="29040" windowHeight="15840" xr2:uid="{230D00FD-D74E-4E7F-B6AD-0424789200CA}"/>
   </bookViews>
   <sheets>
     <sheet name="program" sheetId="1" r:id="rId1"/>
     <sheet name="negatives" sheetId="2" r:id="rId2"/>
-    <sheet name="negatives (backup)" sheetId="3" r:id="rId3"/>
+    <sheet name="solution" sheetId="4" r:id="rId3"/>
+    <sheet name="solution test" sheetId="5" r:id="rId4"/>
+    <sheet name="negatives (backup)" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,12 +29,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="35">
   <si>
     <t>Number of people</t>
   </si>
   <si>
     <t>isWeekend</t>
+  </si>
+  <si>
+    <t>SETTINGS</t>
+  </si>
+  <si>
+    <t>Automatically calculated</t>
+  </si>
+  <si>
+    <t>Allow back-to-back shifts</t>
+  </si>
+  <si>
+    <t>Total Days</t>
+  </si>
+  <si>
+    <t>Balance shifts automatically</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>multiple programs as solutions (3-4)</t>
+  </si>
+  <si>
+    <t>weekend balancing remake</t>
   </si>
   <si>
     <t>ΧΡΙΣΤΟΔΟΥΛΟΥ</t>
@@ -50,7 +76,7 @@
     <t>ΣΟΥΛΙΜΑ</t>
   </si>
   <si>
-    <t>ΜΠΑΚΟΠΟΥΛΟΣ</t>
+    <t>ΜΠΑΜΟΠΟΥΛΟΣ</t>
   </si>
   <si>
     <t>ΚΑΡΑΜΟΛΕΓΚΟΥ</t>
@@ -77,46 +103,37 @@
     <t>ΠΑΝΑΓΟΥΛΑ</t>
   </si>
   <si>
-    <t>Total shifts</t>
-  </si>
-  <si>
-    <t>Total Shifts per person</t>
-  </si>
-  <si>
-    <t>Total shifts alocated per person</t>
-  </si>
-  <si>
-    <t>Allow back-to-back shifts</t>
-  </si>
-  <si>
     <t>Is Junior (cannot work alone)</t>
-  </si>
-  <si>
-    <t>Balance shifts automatically</t>
-  </si>
-  <si>
-    <t>SETTINGS</t>
-  </si>
-  <si>
-    <t>Automatically calculated</t>
-  </si>
-  <si>
-    <t>Total Days</t>
-  </si>
-  <si>
-    <t>ΜΠΑΜΟΠΟΥΛΟΣ</t>
   </si>
   <si>
     <t>Desired shifts per person</t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>multiple programs as solutions (3-4)</t>
+    <t>Total Weekends</t>
   </si>
   <si>
-    <t>weekend balancing remake</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>ΜΠΑΚΟΠΟΥΛΟΣ</t>
+  </si>
+  <si>
+    <t>Total shifts (days)</t>
+  </si>
+  <si>
+    <t>Total shifts (desired per person)</t>
+  </si>
+  <si>
+    <t>Weekend shifts</t>
+  </si>
+  <si>
+    <t>!! These two should be equal !!</t>
   </si>
 </sst>
 </file>
@@ -244,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -256,17 +273,24 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -276,7 +300,8 @@
         <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
@@ -286,7 +311,8 @@
         <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -296,7 +322,52 @@
         <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
@@ -611,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5EEA1A-F88C-432A-B611-29BB32E68D9D}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45612</v>
       </c>
@@ -809,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45613</v>
       </c>
@@ -820,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45614</v>
       </c>
@@ -831,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45615</v>
       </c>
@@ -842,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45616</v>
       </c>
@@ -853,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45617</v>
       </c>
@@ -864,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45618</v>
       </c>
@@ -875,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45619</v>
       </c>
@@ -886,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45620</v>
       </c>
@@ -897,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45621</v>
       </c>
@@ -908,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45622</v>
       </c>
@@ -918,8 +989,11 @@
       <c r="C27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45623</v>
       </c>
@@ -929,8 +1003,11 @@
       <c r="C28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45624</v>
       </c>
@@ -940,8 +1017,11 @@
       <c r="C29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45625</v>
       </c>
@@ -952,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45626</v>
       </c>
@@ -963,72 +1043,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
     </row>
-    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E35" s="10">
         <f>COUNTIF(A2:A32,"&lt;&gt;")</f>
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E36" s="10">
         <f>SUM(B2:B31)</f>
         <v>82</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D37" s="10" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E37" s="10">
         <f>negatives!B37</f>
         <v>82</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D38" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="10">
+        <f>SUMIF(C2:C31, 1, B2:B31)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F36:G37"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1038,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3734B0B9-157B-4360-A5C8-B7323A1492CD}">
   <dimension ref="A1:JA37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,8 +1131,10 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
     <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -1060,49 +1145,49 @@
   <sheetData>
     <row r="1" spans="1:261" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:261" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:261" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45597</v>
       </c>
@@ -1150,7 +1235,7 @@
       </c>
     </row>
     <row r="3" spans="1:261" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>45598</v>
       </c>
       <c r="B3" s="3">
@@ -1442,8 +1527,8 @@
       <c r="IZ3"/>
       <c r="JA3"/>
     </row>
-    <row r="4" spans="1:261" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+    <row r="4" spans="1:261" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>45599</v>
       </c>
       <c r="B4" s="5">
@@ -1923,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:261" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:261" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45604</v>
       </c>
@@ -1971,7 +2056,7 @@
       </c>
     </row>
     <row r="10" spans="1:261" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>45605</v>
       </c>
       <c r="B10" s="3">
@@ -2263,8 +2348,8 @@
       <c r="IZ10"/>
       <c r="JA10"/>
     </row>
-    <row r="11" spans="1:261" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+    <row r="11" spans="1:261" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>45606</v>
       </c>
       <c r="B11" s="5">
@@ -2744,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:261" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:261" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45611</v>
       </c>
@@ -2792,7 +2877,7 @@
       </c>
     </row>
     <row r="17" spans="1:261" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>45612</v>
       </c>
       <c r="B17" s="3">
@@ -3084,8 +3169,8 @@
       <c r="IZ17"/>
       <c r="JA17"/>
     </row>
-    <row r="18" spans="1:261" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+    <row r="18" spans="1:261" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>45613</v>
       </c>
       <c r="B18" s="5">
@@ -3565,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:261" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:261" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45618</v>
       </c>
@@ -3613,7 +3698,7 @@
       </c>
     </row>
     <row r="24" spans="1:261" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>45619</v>
       </c>
       <c r="B24" s="3">
@@ -3905,8 +3990,8 @@
       <c r="IZ24"/>
       <c r="JA24"/>
     </row>
-    <row r="25" spans="1:261" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4">
+    <row r="25" spans="1:261" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
         <v>45620</v>
       </c>
       <c r="B25" s="5">
@@ -4386,7 +4471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:261" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:261" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45625</v>
       </c>
@@ -4433,8 +4518,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:261" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
+    <row r="31" spans="1:261" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
         <v>45626</v>
       </c>
       <c r="B31" s="7">
@@ -4726,14 +4811,17 @@
       <c r="IZ31"/>
       <c r="JA31"/>
     </row>
-    <row r="34" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:261" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="34" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -4780,7 +4868,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36">
         <v>7</v>
@@ -4827,7 +4915,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B37" s="10">
         <f>SUM(B36:O36)</f>
@@ -4836,10 +4924,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:O31 B35:O36">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4849,6 +4937,2544 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76DC296D-CDAA-4ED1-81F3-0E877EF4102F}">
+  <dimension ref="A1:AI31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="32" width="4.77734375" customWidth="1"/>
+    <col min="33" max="34" width="9.109375" customWidth="1"/>
+    <col min="35" max="35" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B1" s="11">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11">
+        <v>8</v>
+      </c>
+      <c r="J1" s="11">
+        <v>9</v>
+      </c>
+      <c r="K1" s="11">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11">
+        <v>11</v>
+      </c>
+      <c r="M1" s="11">
+        <v>12</v>
+      </c>
+      <c r="N1" s="11">
+        <v>13</v>
+      </c>
+      <c r="O1" s="11">
+        <v>14</v>
+      </c>
+      <c r="P1" s="11">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="11">
+        <v>16</v>
+      </c>
+      <c r="R1" s="11">
+        <v>17</v>
+      </c>
+      <c r="S1" s="11">
+        <v>18</v>
+      </c>
+      <c r="T1" s="11">
+        <v>19</v>
+      </c>
+      <c r="U1" s="11">
+        <v>20</v>
+      </c>
+      <c r="V1" s="11">
+        <v>21</v>
+      </c>
+      <c r="W1" s="11">
+        <v>22</v>
+      </c>
+      <c r="X1" s="11">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="11">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="11">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="11">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="11">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="11">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="11">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="11">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="11">
+        <v>1</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>1</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="11">
+        <v>1</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="11">
+        <v>1</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH2">
+        <v>7</v>
+      </c>
+      <c r="AI2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="11">
+        <v>1</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>1</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="11">
+        <v>1</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH3">
+        <v>4</v>
+      </c>
+      <c r="AI3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="11">
+        <v>1</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="11">
+        <v>1</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V4" s="11">
+        <v>1</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y4" s="11">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD4" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH4">
+        <v>7</v>
+      </c>
+      <c r="AI4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="11">
+        <v>1</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X5" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH5">
+        <v>3</v>
+      </c>
+      <c r="AI5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="11">
+        <v>1</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="V6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X6" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA6" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD6" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH6">
+        <v>4</v>
+      </c>
+      <c r="AI6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W7" s="11">
+        <v>1</v>
+      </c>
+      <c r="X7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE7" s="11">
+        <v>1</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH7">
+        <v>4</v>
+      </c>
+      <c r="AI7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="11">
+        <v>1</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="11">
+        <v>1</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="V8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="X8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA8" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH8">
+        <v>4</v>
+      </c>
+      <c r="AI8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="11">
+        <v>1</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="11">
+        <v>1</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S9" s="11">
+        <v>1</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X9" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD9" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH9">
+        <v>7</v>
+      </c>
+      <c r="AI9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="11">
+        <v>1</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="11">
+        <v>1</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10" s="11">
+        <v>1</v>
+      </c>
+      <c r="V10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y10" s="11">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB10" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH10">
+        <v>7</v>
+      </c>
+      <c r="AI10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="11">
+        <v>1</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11" s="11">
+        <v>1</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y11" s="11">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC11" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH11">
+        <v>7</v>
+      </c>
+      <c r="AI11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="11">
+        <v>1</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="11">
+        <v>1</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="11">
+        <v>1</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V12" s="11">
+        <v>1</v>
+      </c>
+      <c r="W12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="X12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH12">
+        <v>7</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="11">
+        <v>1</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="11">
+        <v>1</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="U13" s="11">
+        <v>1</v>
+      </c>
+      <c r="V13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH13">
+        <v>7</v>
+      </c>
+      <c r="AI13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="11">
+        <v>1</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>1</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="U14" s="11">
+        <v>1</v>
+      </c>
+      <c r="V14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH14">
+        <v>7</v>
+      </c>
+      <c r="AI14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="11">
+        <v>1</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S15" s="11">
+        <v>1</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W15" s="11">
+        <v>1</v>
+      </c>
+      <c r="X15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z15" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC15" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH15">
+        <v>7</v>
+      </c>
+      <c r="AI15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:AF15">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F23B7C-A532-4F56-832C-0C78E47E835F}">
+  <dimension ref="A1:AI31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="32" width="4.77734375" customWidth="1"/>
+    <col min="33" max="34" width="9.109375" customWidth="1"/>
+    <col min="35" max="35" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH2">
+        <v>7</v>
+      </c>
+      <c r="AI2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="X3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH3">
+        <v>4</v>
+      </c>
+      <c r="AI3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH4">
+        <v>7</v>
+      </c>
+      <c r="AI4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>3</v>
+      </c>
+      <c r="AI5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>28</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <v>4</v>
+      </c>
+      <c r="AI6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
+        <v>28</v>
+      </c>
+      <c r="U7" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>4</v>
+      </c>
+      <c r="AI7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <v>4</v>
+      </c>
+      <c r="AI8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
+        <v>28</v>
+      </c>
+      <c r="U9" t="s">
+        <v>28</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>7</v>
+      </c>
+      <c r="AI9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" t="s">
+        <v>28</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <v>7</v>
+      </c>
+      <c r="AI10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>28</v>
+      </c>
+      <c r="T11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>7</v>
+      </c>
+      <c r="AI11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" t="s">
+        <v>28</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12" t="s">
+        <v>28</v>
+      </c>
+      <c r="X12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC12">
+        <v>1</v>
+      </c>
+      <c r="AH12">
+        <v>7</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="X13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AE13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <v>7</v>
+      </c>
+      <c r="AI13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AE14">
+        <v>1</v>
+      </c>
+      <c r="AH14">
+        <v>7</v>
+      </c>
+      <c r="AI14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15" t="s">
+        <v>28</v>
+      </c>
+      <c r="U15" t="s">
+        <v>28</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AH15">
+        <v>7</v>
+      </c>
+      <c r="AI15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:AF15">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6791206B-FCA3-400E-91E6-C25B98570E8E}">
   <dimension ref="A1:O31"/>
   <sheetViews>
@@ -4859,54 +7485,55 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="9.109375" customWidth="1"/>
     <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45597</v>
       </c>
@@ -5000,7 +7627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45599</v>
       </c>
@@ -5235,7 +7862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45604</v>
       </c>
@@ -5329,7 +7956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45606</v>
       </c>
@@ -5564,7 +8191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45611</v>
       </c>
@@ -5658,7 +8285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>45613</v>
       </c>
@@ -5893,7 +8520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45618</v>
       </c>
@@ -5987,7 +8614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>45620</v>
       </c>
@@ -6222,7 +8849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45625</v>
       </c>
@@ -6269,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>45626</v>
       </c>

</xml_diff>